<commit_message>
Created code to grab locations(need to clean up data)
</commit_message>
<xml_diff>
--- a/Consolidated_Estimator_Worksheet.xlsx
+++ b/Consolidated_Estimator_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00523D7B-4653-41D7-B27B-EF22C24658EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{0587D576-A4F2-4999-AFF1-79ADD1275623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="32" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="30" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
@@ -49,15 +49,16 @@
     <sheet name="Consolidated_Clean" sheetId="34" r:id="rId34"/>
     <sheet name="Working_Table12" sheetId="35" r:id="rId35"/>
     <sheet name="Cleaned_Data12" sheetId="36" r:id="rId36"/>
+    <sheet name="Location_Table" sheetId="37" r:id="rId37"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">Consolidated_Clean!$A$2:$E$540</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId37"/>
-    <pivotCache cacheId="1" r:id="rId38"/>
-    <pivotCache cacheId="2" r:id="rId39"/>
+    <pivotCache cacheId="0" r:id="rId38"/>
+    <pivotCache cacheId="1" r:id="rId39"/>
+    <pivotCache cacheId="2" r:id="rId40"/>
   </pivotCaches>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -76,8 +77,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6033" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6065" uniqueCount="214">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -664,7 +687,61 @@
     <t>https://www.supplyworks.com/Sku/2487704/southwire-250-ft-122-solid-romex-simpull-cu-nm-b-wg-wire-032886163050-28828255</t>
   </si>
   <si>
+    <t>Vendor</t>
+  </si>
+  <si>
     <t>11/03/2022 10:49:30</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>['2455 Paces Ferry Rd SE, Atlanta, GA 30339']</t>
+  </si>
+  <si>
+    <t>["1000 Lowe's Blvd. Mooresville NC 28117"]</t>
+  </si>
+  <si>
+    <t>['Kankakee, 1290 N Hobbie Ave. HQ']</t>
+  </si>
+  <si>
+    <t>['6260 Abbott Dr, Omaha, Nebraska, 68110']</t>
+  </si>
+  <si>
+    <t>['Jacksonville, Florida']</t>
+  </si>
+  <si>
+    <t>['4777 Menard Drive Eau Claire, Wisconsin 54703 USA']</t>
+  </si>
+  <si>
+    <t>['the National Landing neighborhood of Arlington']</t>
+  </si>
+  <si>
+    <t>['28 Biopolis Road Singapore 138568']</t>
+  </si>
+  <si>
+    <t>['Steel City', 'connector', 'EMT conduit', 'Connector', 'steel']</t>
+  </si>
+  <si>
+    <t>['San Jose, CA. 2025 Hamilton Avenue San Jose, California 95125 USA']</t>
+  </si>
+  <si>
+    <t>['Grand Rapids, Minnesota, United States']</t>
+  </si>
+  <si>
+    <t>['Bentonville, Arkansas']</t>
+  </si>
+  <si>
+    <t>['574 Road 11, Schuyler, Nebraska, 68661, United States']</t>
+  </si>
+  <si>
+    <t>['1431 7th St Ste 204, Santa Monica, California, 90401']</t>
+  </si>
+  <si>
+    <t>Unique supplier names</t>
+  </si>
+  <si>
+    <t>Unique Suppliers</t>
   </si>
 </sst>
 </file>
@@ -676,7 +753,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="dddd"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -926,6 +1003,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -995,7 +1077,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1631,12 +1713,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1844,6 +1941,13 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1895,7 +1999,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17849,13 +17955,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="124"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="127"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -17878,14 +17984,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="125" t="s">
+      <c r="E10" s="128" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="127" t="s">
+      <c r="G10" s="130" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -17905,11 +18011,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="126"/>
+      <c r="E11" s="129"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="116"/>
+      <c r="G11" s="119"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -17921,59 +18027,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="129">
+      <c r="B12" s="132">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="129">
+      <c r="C12" s="132">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="129">
+      <c r="D12" s="132">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="129">
+      <c r="E12" s="132">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="129">
+      <c r="F12" s="132">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="117">
+      <c r="G12" s="120">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="H12" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="116"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
+      <c r="A13" s="119"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -18038,10 +18144,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="121"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -18058,10 +18164,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -18078,15 +18184,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="122"/>
-      <c r="H20" s="122"/>
-      <c r="I20" s="122"/>
-      <c r="J20" s="122"/>
-      <c r="K20" s="122"/>
+      <c r="C20" s="124"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="125"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
+      <c r="K20" s="125"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -18098,10 +18204,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="113"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -18131,14 +18237,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="115" t="s">
+      <c r="C23" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -18151,12 +18257,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -18169,12 +18275,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="116"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="119"/>
+      <c r="H25" s="119"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -27831,8 +27937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27842,10 +27948,10 @@
     <col min="3" max="3" width="47.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" style="111" customWidth="1"/>
+    <col min="6" max="6" width="50.06640625" style="111" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="70" t="s">
         <v>24</v>
       </c>
@@ -27853,7 +27959,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="D1" s="70" t="s">
         <v>84</v>
@@ -27861,8 +27967,11 @@
       <c r="E1" s="110" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="111" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -27876,11 +27985,15 @@
         <v>87</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="0">TEXT(D2,"dddd")</f>
+        <f t="shared" ref="E2:E65" si="0">TEXT(D2,"dddd")</f>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" s="111" t="str" cm="1">
+        <f t="array" ref="F2:F11">_xlfn.UNIQUE(C2:C209)</f>
+        <v>gordonelectricsupply</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -27897,8 +28010,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" s="111" t="str">
+        <v>ebarnett</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -27915,8 +28031,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" s="111" t="str">
+        <v>amazon</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -27933,8 +28052,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" s="111" t="str">
+        <v>pinterest</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -27951,8 +28073,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" s="111" t="str">
+        <v>homedepot</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -27969,8 +28094,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" s="111" t="str">
+        <v>ebay</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -27987,8 +28115,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" s="111" t="str">
+        <v>dkhardware</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -28005,8 +28136,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" s="111" t="str">
+        <v>com/p/halex-screw-emt-conduit-connector-051411262723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -28023,8 +28157,11 @@
         <f t="shared" si="0"/>
         <v>Sunday</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" s="111" t="str">
+        <v>com/p/steel-city-emt-conduit-connector-785991183801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -28041,8 +28178,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" s="111" t="str">
+        <v>qcsupply</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -28060,7 +28200,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -28078,7 +28218,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -28096,7 +28236,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -28114,7 +28254,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -28452,7 +28592,7 @@
         <v>152</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E65" si="1">TEXT(D34,"dddd")</f>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28470,7 +28610,7 @@
         <v>152</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28488,7 +28628,7 @@
         <v>152</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28506,7 +28646,7 @@
         <v>152</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28524,7 +28664,7 @@
         <v>152</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28542,7 +28682,7 @@
         <v>152</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28560,7 +28700,7 @@
         <v>152</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28578,7 +28718,7 @@
         <v>152</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28596,7 +28736,7 @@
         <v>152</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28614,7 +28754,7 @@
         <v>152</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28632,7 +28772,7 @@
         <v>152</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28650,7 +28790,7 @@
         <v>152</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28668,7 +28808,7 @@
         <v>152</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28686,7 +28826,7 @@
         <v>152</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28704,7 +28844,7 @@
         <v>152</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28722,7 +28862,7 @@
         <v>152</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
     </row>
@@ -28740,7 +28880,7 @@
         <v>156</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28758,7 +28898,7 @@
         <v>156</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28776,7 +28916,7 @@
         <v>156</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28794,7 +28934,7 @@
         <v>156</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28812,7 +28952,7 @@
         <v>156</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28830,7 +28970,7 @@
         <v>156</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28848,7 +28988,7 @@
         <v>156</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28866,7 +29006,7 @@
         <v>156</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28884,7 +29024,7 @@
         <v>156</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28902,7 +29042,7 @@
         <v>156</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28920,7 +29060,7 @@
         <v>156</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28938,7 +29078,7 @@
         <v>156</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28956,7 +29096,7 @@
         <v>156</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28974,7 +29114,7 @@
         <v>156</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -28992,7 +29132,7 @@
         <v>156</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -29010,7 +29150,7 @@
         <v>157</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -29028,7 +29168,7 @@
         <v>163</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E97" si="2">TEXT(D66,"dddd")</f>
+        <f t="shared" ref="E66:E129" si="1">TEXT(D66,"dddd")</f>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29046,7 +29186,7 @@
         <v>163</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29064,7 +29204,7 @@
         <v>163</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29082,7 +29222,7 @@
         <v>163</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29100,7 +29240,7 @@
         <v>163</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29118,7 +29258,7 @@
         <v>156</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -29136,7 +29276,7 @@
         <v>163</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29154,7 +29294,7 @@
         <v>163</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29172,7 +29312,7 @@
         <v>163</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29190,7 +29330,7 @@
         <v>163</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29208,7 +29348,7 @@
         <v>163</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29226,7 +29366,7 @@
         <v>163</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29244,7 +29384,7 @@
         <v>163</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29262,7 +29402,7 @@
         <v>163</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29280,7 +29420,7 @@
         <v>156</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -29298,7 +29438,7 @@
         <v>163</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -29316,7 +29456,7 @@
         <v>168</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29334,7 +29474,7 @@
         <v>168</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29352,7 +29492,7 @@
         <v>168</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29370,7 +29510,7 @@
         <v>168</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29388,7 +29528,7 @@
         <v>168</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29406,7 +29546,7 @@
         <v>168</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29424,7 +29564,7 @@
         <v>168</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29442,7 +29582,7 @@
         <v>168</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29460,7 +29600,7 @@
         <v>168</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29478,7 +29618,7 @@
         <v>168</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29496,7 +29636,7 @@
         <v>168</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29514,7 +29654,7 @@
         <v>168</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29532,7 +29672,7 @@
         <v>168</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29550,7 +29690,7 @@
         <v>168</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29568,7 +29708,7 @@
         <v>168</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29586,7 +29726,7 @@
         <v>168</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29604,7 +29744,7 @@
         <v>171</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" ref="E98:E129" si="3">TEXT(D98,"dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29622,7 +29762,7 @@
         <v>171</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29640,7 +29780,7 @@
         <v>171</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29658,7 +29798,7 @@
         <v>171</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29676,7 +29816,7 @@
         <v>171</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29694,7 +29834,7 @@
         <v>171</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29712,7 +29852,7 @@
         <v>171</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29730,7 +29870,7 @@
         <v>171</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29748,7 +29888,7 @@
         <v>168</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
     </row>
@@ -29766,7 +29906,7 @@
         <v>171</v>
       </c>
       <c r="E107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29784,7 +29924,7 @@
         <v>171</v>
       </c>
       <c r="E108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29802,7 +29942,7 @@
         <v>171</v>
       </c>
       <c r="E109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29820,7 +29960,7 @@
         <v>171</v>
       </c>
       <c r="E110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29838,7 +29978,7 @@
         <v>171</v>
       </c>
       <c r="E111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29856,7 +29996,7 @@
         <v>171</v>
       </c>
       <c r="E112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29874,7 +30014,7 @@
         <v>171</v>
       </c>
       <c r="E113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
     </row>
@@ -29892,7 +30032,7 @@
         <v>176</v>
       </c>
       <c r="E114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -29910,7 +30050,7 @@
         <v>176</v>
       </c>
       <c r="E115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -29928,7 +30068,7 @@
         <v>176</v>
       </c>
       <c r="E116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -29946,7 +30086,7 @@
         <v>176</v>
       </c>
       <c r="E117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -29964,7 +30104,7 @@
         <v>176</v>
       </c>
       <c r="E118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -29982,7 +30122,7 @@
         <v>176</v>
       </c>
       <c r="E119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30000,7 +30140,7 @@
         <v>176</v>
       </c>
       <c r="E120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30018,7 +30158,7 @@
         <v>176</v>
       </c>
       <c r="E121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30036,7 +30176,7 @@
         <v>176</v>
       </c>
       <c r="E122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30054,7 +30194,7 @@
         <v>176</v>
       </c>
       <c r="E123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30072,7 +30212,7 @@
         <v>176</v>
       </c>
       <c r="E124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30090,7 +30230,7 @@
         <v>176</v>
       </c>
       <c r="E125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30108,7 +30248,7 @@
         <v>176</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30126,7 +30266,7 @@
         <v>176</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30144,7 +30284,7 @@
         <v>176</v>
       </c>
       <c r="E128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30162,7 +30302,7 @@
         <v>176</v>
       </c>
       <c r="E129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
     </row>
@@ -30180,7 +30320,7 @@
         <v>180</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" ref="E130:E161" si="4">TEXT(D130,"dddd")</f>
+        <f t="shared" ref="E130:E193" si="2">TEXT(D130,"dddd")</f>
         <v>Sunday</v>
       </c>
     </row>
@@ -30198,7 +30338,7 @@
         <v>180</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30216,7 +30356,7 @@
         <v>180</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30234,7 +30374,7 @@
         <v>180</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30252,7 +30392,7 @@
         <v>180</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30270,7 +30410,7 @@
         <v>180</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30288,7 +30428,7 @@
         <v>180</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30306,7 +30446,7 @@
         <v>180</v>
       </c>
       <c r="E137" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30324,7 +30464,7 @@
         <v>180</v>
       </c>
       <c r="E138" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30342,7 +30482,7 @@
         <v>180</v>
       </c>
       <c r="E139" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30360,7 +30500,7 @@
         <v>180</v>
       </c>
       <c r="E140" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30378,7 +30518,7 @@
         <v>180</v>
       </c>
       <c r="E141" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30396,7 +30536,7 @@
         <v>180</v>
       </c>
       <c r="E142" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30414,7 +30554,7 @@
         <v>180</v>
       </c>
       <c r="E143" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30432,7 +30572,7 @@
         <v>180</v>
       </c>
       <c r="E144" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30450,7 +30590,7 @@
         <v>180</v>
       </c>
       <c r="E145" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Sunday</v>
       </c>
     </row>
@@ -30468,7 +30608,7 @@
         <v>183</v>
       </c>
       <c r="E146" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30486,7 +30626,7 @@
         <v>183</v>
       </c>
       <c r="E147" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30504,7 +30644,7 @@
         <v>183</v>
       </c>
       <c r="E148" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30522,7 +30662,7 @@
         <v>183</v>
       </c>
       <c r="E149" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30540,7 +30680,7 @@
         <v>183</v>
       </c>
       <c r="E150" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30558,7 +30698,7 @@
         <v>183</v>
       </c>
       <c r="E151" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30576,7 +30716,7 @@
         <v>183</v>
       </c>
       <c r="E152" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30594,7 +30734,7 @@
         <v>183</v>
       </c>
       <c r="E153" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30612,7 +30752,7 @@
         <v>183</v>
       </c>
       <c r="E154" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30630,7 +30770,7 @@
         <v>183</v>
       </c>
       <c r="E155" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30648,7 +30788,7 @@
         <v>183</v>
       </c>
       <c r="E156" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30666,7 +30806,7 @@
         <v>183</v>
       </c>
       <c r="E157" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30684,7 +30824,7 @@
         <v>183</v>
       </c>
       <c r="E158" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30702,7 +30842,7 @@
         <v>183</v>
       </c>
       <c r="E159" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30720,7 +30860,7 @@
         <v>183</v>
       </c>
       <c r="E160" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30738,7 +30878,7 @@
         <v>183</v>
       </c>
       <c r="E161" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>Monday</v>
       </c>
     </row>
@@ -30756,7 +30896,7 @@
         <v>185</v>
       </c>
       <c r="E162" t="str">
-        <f t="shared" ref="E162:E209" si="5">TEXT(D162,"dddd")</f>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30774,7 +30914,7 @@
         <v>185</v>
       </c>
       <c r="E163" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30792,7 +30932,7 @@
         <v>185</v>
       </c>
       <c r="E164" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30810,7 +30950,7 @@
         <v>185</v>
       </c>
       <c r="E165" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30828,7 +30968,7 @@
         <v>185</v>
       </c>
       <c r="E166" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30846,7 +30986,7 @@
         <v>185</v>
       </c>
       <c r="E167" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30864,7 +31004,7 @@
         <v>185</v>
       </c>
       <c r="E168" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30882,7 +31022,7 @@
         <v>185</v>
       </c>
       <c r="E169" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30900,7 +31040,7 @@
         <v>185</v>
       </c>
       <c r="E170" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30918,7 +31058,7 @@
         <v>185</v>
       </c>
       <c r="E171" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30936,7 +31076,7 @@
         <v>185</v>
       </c>
       <c r="E172" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30954,7 +31094,7 @@
         <v>185</v>
       </c>
       <c r="E173" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30972,7 +31112,7 @@
         <v>185</v>
       </c>
       <c r="E174" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -30990,7 +31130,7 @@
         <v>185</v>
       </c>
       <c r="E175" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -31008,7 +31148,7 @@
         <v>185</v>
       </c>
       <c r="E176" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -31026,7 +31166,7 @@
         <v>185</v>
       </c>
       <c r="E177" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Tuesday</v>
       </c>
     </row>
@@ -31044,7 +31184,7 @@
         <v>190</v>
       </c>
       <c r="E178" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31062,7 +31202,7 @@
         <v>190</v>
       </c>
       <c r="E179" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31080,7 +31220,7 @@
         <v>191</v>
       </c>
       <c r="E180" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31098,7 +31238,7 @@
         <v>191</v>
       </c>
       <c r="E181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31116,7 +31256,7 @@
         <v>191</v>
       </c>
       <c r="E182" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31134,7 +31274,7 @@
         <v>191</v>
       </c>
       <c r="E183" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31152,7 +31292,7 @@
         <v>191</v>
       </c>
       <c r="E184" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31170,7 +31310,7 @@
         <v>191</v>
       </c>
       <c r="E185" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31188,7 +31328,7 @@
         <v>191</v>
       </c>
       <c r="E186" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31206,7 +31346,7 @@
         <v>191</v>
       </c>
       <c r="E187" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31224,7 +31364,7 @@
         <v>191</v>
       </c>
       <c r="E188" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31242,7 +31382,7 @@
         <v>191</v>
       </c>
       <c r="E189" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31260,7 +31400,7 @@
         <v>191</v>
       </c>
       <c r="E190" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31278,7 +31418,7 @@
         <v>191</v>
       </c>
       <c r="E191" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
@@ -31296,11 +31436,11 @@
         <v>191</v>
       </c>
       <c r="E192" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>114</v>
       </c>
@@ -31314,11 +31454,11 @@
         <v>191</v>
       </c>
       <c r="E193" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>Wednesday</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>85</v>
       </c>
@@ -31329,15 +31469,14 @@
         <v>57</v>
       </c>
       <c r="D194" t="s">
-        <v>195</v>
-      </c>
-      <c r="E194" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E194" s="113" t="str">
+        <f t="shared" ref="E194:E257" si="3">TEXT(D194,"dddd")</f>
         <v>Thursday</v>
       </c>
-      <c r="F194"/>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>88</v>
       </c>
@@ -31348,15 +31487,14 @@
         <v>55</v>
       </c>
       <c r="D195" t="s">
-        <v>195</v>
-      </c>
-      <c r="E195" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E195" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F195"/>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>73</v>
       </c>
@@ -31367,15 +31505,14 @@
         <v>58</v>
       </c>
       <c r="D196" t="s">
-        <v>195</v>
-      </c>
-      <c r="E196" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E196" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F196"/>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>91</v>
       </c>
@@ -31386,15 +31523,14 @@
         <v>49</v>
       </c>
       <c r="D197" t="s">
-        <v>195</v>
-      </c>
-      <c r="E197" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E197" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F197"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>93</v>
       </c>
@@ -31405,15 +31541,14 @@
         <v>58</v>
       </c>
       <c r="D198" t="s">
-        <v>195</v>
-      </c>
-      <c r="E198" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E198" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F198"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>95</v>
       </c>
@@ -31424,15 +31559,14 @@
         <v>58</v>
       </c>
       <c r="D199" t="s">
-        <v>195</v>
-      </c>
-      <c r="E199" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E199" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F199"/>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>97</v>
       </c>
@@ -31443,15 +31577,14 @@
         <v>49</v>
       </c>
       <c r="D200" t="s">
-        <v>195</v>
-      </c>
-      <c r="E200" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E200" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F200"/>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>98</v>
       </c>
@@ -31462,15 +31595,14 @@
         <v>49</v>
       </c>
       <c r="D201" t="s">
-        <v>195</v>
-      </c>
-      <c r="E201" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E201" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F201"/>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>100</v>
       </c>
@@ -31481,15 +31613,14 @@
         <v>52</v>
       </c>
       <c r="D202" t="s">
-        <v>195</v>
-      </c>
-      <c r="E202" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E202" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F202"/>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>102</v>
       </c>
@@ -31500,15 +31631,14 @@
         <v>49</v>
       </c>
       <c r="D203" t="s">
-        <v>195</v>
-      </c>
-      <c r="E203" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E203" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F203"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>104</v>
       </c>
@@ -31519,15 +31649,14 @@
         <v>56</v>
       </c>
       <c r="D204" t="s">
-        <v>195</v>
-      </c>
-      <c r="E204" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E204" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F204"/>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>106</v>
       </c>
@@ -31538,15 +31667,14 @@
         <v>58</v>
       </c>
       <c r="D205" t="s">
-        <v>195</v>
-      </c>
-      <c r="E205" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E205" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F205"/>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>108</v>
       </c>
@@ -31557,15 +31685,14 @@
         <v>58</v>
       </c>
       <c r="D206" t="s">
-        <v>195</v>
-      </c>
-      <c r="E206" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E206" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F206"/>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>110</v>
       </c>
@@ -31576,15 +31703,14 @@
         <v>49</v>
       </c>
       <c r="D207" t="s">
-        <v>195</v>
-      </c>
-      <c r="E207" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E207" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F207"/>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>112</v>
       </c>
@@ -31595,15 +31721,14 @@
         <v>49</v>
       </c>
       <c r="D208" t="s">
-        <v>195</v>
-      </c>
-      <c r="E208" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E208" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F208"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>114</v>
       </c>
@@ -31614,13 +31739,12 @@
         <v>49</v>
       </c>
       <c r="D209" t="s">
-        <v>195</v>
-      </c>
-      <c r="E209" s="136" t="str">
-        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="E209" s="113" t="str">
+        <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="F209"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31630,10 +31754,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
-  <dimension ref="A1:E584"/>
+  <dimension ref="A1:F584"/>
   <sheetViews>
-    <sheetView topLeftCell="A554" workbookViewId="0">
-      <selection activeCell="E540" sqref="E540:E584"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31643,9 +31767,10 @@
     <col min="3" max="3" width="47.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="70" t="s">
         <v>24</v>
       </c>
@@ -31653,7 +31778,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="D1" s="70" t="s">
         <v>84</v>
@@ -31661,8 +31786,11 @@
       <c r="E1" s="83" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="139" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -31679,8 +31807,12 @@
         <f t="shared" ref="E2:E65" si="0">TEXT(D2,"dddd")</f>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="str" cm="1">
+        <f t="array" ref="F2:F26">_xlfn.UNIQUE(C2:C584)</f>
+        <v>homedepot</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -31697,8 +31829,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="str">
+        <v>lowes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -31715,8 +31850,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="str">
+        <v>gordonelectricsupply</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -31733,8 +31871,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="str">
+        <v>supplyworks</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -31751,8 +31892,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="str">
+        <v>ebarnett</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -31769,8 +31913,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="str">
+        <v>linemen-tools</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -31787,8 +31934,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" t="str">
+        <v>dkhardware</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -31805,8 +31955,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="str">
+        <v>amazon</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -31823,8 +31976,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" t="str">
+        <v>wilmar</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -31841,8 +31997,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" t="str">
+        <v>pinterest</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -31859,8 +32018,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="str">
+        <v>ebay</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -31877,8 +32039,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="str">
+        <v>com/p/solid-romex-simpull-cu-nm-b-wire-032886163005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -31895,8 +32060,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="str">
+        <v>qcsupply</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -31913,8 +32081,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F15" t="str">
+        <v>cooper-electric</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -31931,8 +32102,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="str">
+        <v>truevalue</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -31949,8 +32123,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="str">
+        <v>landmsupply</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -31967,8 +32144,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="str">
+        <v>superarbor</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -31985,8 +32165,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="str">
+        <v>menards</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -32003,8 +32186,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="str">
+        <v>mecampbell</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -32021,8 +32207,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" t="str">
+        <v>socalelectric</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -32039,8 +32228,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" t="str">
+        <v>wireandcableyourway</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -32057,8 +32249,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" t="str">
+        <v>com/p/halex-screw-emt-conduit-connector-051411262723</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -32075,8 +32270,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="str">
+        <v>rona</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -32093,8 +32291,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25" t="str">
+        <v>com/p/steel-city-emt-conduit-connector-785991183801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -32111,8 +32312,11 @@
         <f t="shared" si="0"/>
         <v>Saturday</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26" t="str">
+        <v>walmart</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -32130,7 +32334,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -32148,7 +32352,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -32166,7 +32370,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -32184,7 +32388,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -32202,7 +32406,7 @@
         <v>Saturday</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -41375,7 +41579,7 @@
         <v>57</v>
       </c>
       <c r="D541" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E541" t="str">
         <f t="shared" si="8"/>
@@ -41393,7 +41597,7 @@
         <v>58</v>
       </c>
       <c r="D542" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E542" t="str">
         <f t="shared" si="8"/>
@@ -41411,7 +41615,7 @@
         <v>55</v>
       </c>
       <c r="D543" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E543" t="str">
         <f t="shared" si="8"/>
@@ -41429,7 +41633,7 @@
         <v>57</v>
       </c>
       <c r="D544" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E544" t="str">
         <f t="shared" si="8"/>
@@ -41447,7 +41651,7 @@
         <v>58</v>
       </c>
       <c r="D545" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E545" t="str">
         <f t="shared" si="8"/>
@@ -41465,7 +41669,7 @@
         <v>71</v>
       </c>
       <c r="D546" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E546" t="str">
         <f t="shared" si="8"/>
@@ -41483,7 +41687,7 @@
         <v>58</v>
       </c>
       <c r="D547" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E547" t="str">
         <f t="shared" si="8"/>
@@ -41501,7 +41705,7 @@
         <v>49</v>
       </c>
       <c r="D548" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E548" t="str">
         <f t="shared" si="8"/>
@@ -41519,7 +41723,7 @@
         <v>58</v>
       </c>
       <c r="D549" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E549" t="str">
         <f t="shared" si="8"/>
@@ -41537,7 +41741,7 @@
         <v>69</v>
       </c>
       <c r="D550" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E550" t="str">
         <f t="shared" si="8"/>
@@ -41555,7 +41759,7 @@
         <v>61</v>
       </c>
       <c r="D551" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E551" t="str">
         <f t="shared" si="8"/>
@@ -41573,7 +41777,7 @@
         <v>64</v>
       </c>
       <c r="D552" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E552" t="str">
         <f t="shared" si="8"/>
@@ -41591,7 +41795,7 @@
         <v>58</v>
       </c>
       <c r="D553" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E553" t="str">
         <f t="shared" si="8"/>
@@ -41609,7 +41813,7 @@
         <v>58</v>
       </c>
       <c r="D554" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E554" t="str">
         <f t="shared" si="8"/>
@@ -41627,7 +41831,7 @@
         <v>49</v>
       </c>
       <c r="D555" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E555" t="str">
         <f t="shared" si="8"/>
@@ -41645,7 +41849,7 @@
         <v>61</v>
       </c>
       <c r="D556" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E556" t="str">
         <f t="shared" si="8"/>
@@ -41663,7 +41867,7 @@
         <v>71</v>
       </c>
       <c r="D557" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E557" t="str">
         <f t="shared" si="8"/>
@@ -41681,7 +41885,7 @@
         <v>58</v>
       </c>
       <c r="D558" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E558" t="str">
         <f t="shared" si="8"/>
@@ -41699,7 +41903,7 @@
         <v>61</v>
       </c>
       <c r="D559" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E559" t="str">
         <f t="shared" si="8"/>
@@ -41717,7 +41921,7 @@
         <v>49</v>
       </c>
       <c r="D560" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E560" t="str">
         <f t="shared" si="8"/>
@@ -41735,7 +41939,7 @@
         <v>58</v>
       </c>
       <c r="D561" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E561" t="str">
         <f t="shared" si="8"/>
@@ -41753,7 +41957,7 @@
         <v>52</v>
       </c>
       <c r="D562" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E562" t="str">
         <f t="shared" si="8"/>
@@ -41771,7 +41975,7 @@
         <v>58</v>
       </c>
       <c r="D563" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E563" t="str">
         <f t="shared" si="8"/>
@@ -41789,7 +41993,7 @@
         <v>49</v>
       </c>
       <c r="D564" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E564" t="str">
         <f t="shared" si="8"/>
@@ -41807,7 +42011,7 @@
         <v>61</v>
       </c>
       <c r="D565" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E565" t="str">
         <f t="shared" si="8"/>
@@ -41825,7 +42029,7 @@
         <v>56</v>
       </c>
       <c r="D566" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E566" t="str">
         <f t="shared" si="8"/>
@@ -41843,7 +42047,7 @@
         <v>59</v>
       </c>
       <c r="D567" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E567" t="str">
         <f t="shared" si="8"/>
@@ -41861,7 +42065,7 @@
         <v>58</v>
       </c>
       <c r="D568" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E568" t="str">
         <f t="shared" si="8"/>
@@ -41879,7 +42083,7 @@
         <v>61</v>
       </c>
       <c r="D569" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E569" t="str">
         <f t="shared" si="8"/>
@@ -41897,7 +42101,7 @@
         <v>56</v>
       </c>
       <c r="D570" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E570" t="str">
         <f t="shared" si="8"/>
@@ -41915,7 +42119,7 @@
         <v>192</v>
       </c>
       <c r="D571" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E571" t="str">
         <f t="shared" si="8"/>
@@ -41933,7 +42137,7 @@
         <v>58</v>
       </c>
       <c r="D572" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E572" t="str">
         <f t="shared" si="8"/>
@@ -41951,7 +42155,7 @@
         <v>61</v>
       </c>
       <c r="D573" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E573" t="str">
         <f t="shared" si="8"/>
@@ -41969,7 +42173,7 @@
         <v>58</v>
       </c>
       <c r="D574" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E574" t="str">
         <f t="shared" si="8"/>
@@ -41987,7 +42191,7 @@
         <v>61</v>
       </c>
       <c r="D575" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E575" t="str">
         <f t="shared" si="8"/>
@@ -42005,7 +42209,7 @@
         <v>65</v>
       </c>
       <c r="D576" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E576" t="str">
         <f t="shared" si="8"/>
@@ -42023,7 +42227,7 @@
         <v>58</v>
       </c>
       <c r="D577" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E577" t="str">
         <f t="shared" si="8"/>
@@ -42041,10 +42245,10 @@
         <v>49</v>
       </c>
       <c r="D578" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E578" t="str">
-        <f t="shared" ref="E578:E584" si="9">TEXT(D578,"dddd")</f>
+        <f t="shared" ref="E578:E641" si="9">TEXT(D578,"dddd")</f>
         <v>Thursday</v>
       </c>
     </row>
@@ -42059,7 +42263,7 @@
         <v>56</v>
       </c>
       <c r="D579" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E579" t="str">
         <f t="shared" si="9"/>
@@ -42077,7 +42281,7 @@
         <v>58</v>
       </c>
       <c r="D580" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E580" t="str">
         <f t="shared" si="9"/>
@@ -42095,7 +42299,7 @@
         <v>49</v>
       </c>
       <c r="D581" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E581" t="str">
         <f t="shared" si="9"/>
@@ -42113,7 +42317,7 @@
         <v>56</v>
       </c>
       <c r="D582" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E582" t="str">
         <f t="shared" si="9"/>
@@ -42131,7 +42335,7 @@
         <v>58</v>
       </c>
       <c r="D583" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E583" t="str">
         <f t="shared" si="9"/>
@@ -42149,7 +42353,7 @@
         <v>49</v>
       </c>
       <c r="D584" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E584" t="str">
         <f t="shared" si="9"/>
@@ -42167,7 +42371,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -42187,8 +42391,8 @@
       <c r="C1" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="112" t="s">
-        <v>27</v>
+      <c r="D1" s="114" t="s">
+        <v>195</v>
       </c>
       <c r="E1" s="112" t="s">
         <v>83</v>
@@ -42214,7 +42418,7 @@
         <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -42234,7 +42438,7 @@
         <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -42254,7 +42458,7 @@
         <v>141</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -42274,7 +42478,7 @@
         <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -42294,7 +42498,7 @@
         <v>177</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -42314,7 +42518,7 @@
         <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -42334,7 +42538,7 @@
         <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -42354,7 +42558,7 @@
         <v>184</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -42374,7 +42578,7 @@
         <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -42394,7 +42598,7 @@
         <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -42414,7 +42618,7 @@
         <v>186</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -42434,7 +42638,7 @@
         <v>129</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -42454,7 +42658,7 @@
         <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -42474,7 +42678,7 @@
         <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -42494,7 +42698,7 @@
         <v>140</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -42514,7 +42718,7 @@
         <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -42526,8 +42730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -42547,8 +42751,8 @@
       <c r="C1" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="112" t="s">
-        <v>27</v>
+      <c r="D1" s="114" t="s">
+        <v>195</v>
       </c>
       <c r="E1" s="112" t="s">
         <v>83</v>
@@ -42574,7 +42778,7 @@
         <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -42594,7 +42798,7 @@
         <v>119</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -42614,7 +42818,7 @@
         <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -42634,7 +42838,7 @@
         <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -42654,7 +42858,7 @@
         <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -42674,7 +42878,7 @@
         <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -42694,7 +42898,7 @@
         <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -42714,7 +42918,7 @@
         <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -42734,7 +42938,7 @@
         <v>177</v>
       </c>
       <c r="F10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -42754,7 +42958,7 @@
         <v>153</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -42774,7 +42978,7 @@
         <v>164</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -42794,7 +42998,7 @@
         <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -42814,7 +43018,7 @@
         <v>96</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -42834,7 +43038,7 @@
         <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -42854,7 +43058,7 @@
         <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -42874,7 +43078,7 @@
         <v>125</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -42894,7 +43098,7 @@
         <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -42914,7 +43118,7 @@
         <v>99</v>
       </c>
       <c r="F19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -42934,7 +43138,7 @@
         <v>146</v>
       </c>
       <c r="F20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -42954,7 +43158,7 @@
         <v>184</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -42974,7 +43178,7 @@
         <v>101</v>
       </c>
       <c r="F22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -42994,7 +43198,7 @@
         <v>181</v>
       </c>
       <c r="F23" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -43014,7 +43218,7 @@
         <v>155</v>
       </c>
       <c r="F24" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -43034,7 +43238,7 @@
         <v>126</v>
       </c>
       <c r="F25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -43054,7 +43258,7 @@
         <v>182</v>
       </c>
       <c r="F26" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -43074,7 +43278,7 @@
         <v>147</v>
       </c>
       <c r="F27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -43094,7 +43298,7 @@
         <v>148</v>
       </c>
       <c r="F28" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -43114,7 +43318,7 @@
         <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -43134,7 +43338,7 @@
         <v>128</v>
       </c>
       <c r="F30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -43154,7 +43358,7 @@
         <v>186</v>
       </c>
       <c r="F31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -43174,7 +43378,7 @@
         <v>193</v>
       </c>
       <c r="F32" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -43194,7 +43398,7 @@
         <v>129</v>
       </c>
       <c r="F33" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -43214,7 +43418,7 @@
         <v>149</v>
       </c>
       <c r="F34" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -43234,7 +43438,7 @@
         <v>109</v>
       </c>
       <c r="F35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -43254,7 +43458,7 @@
         <v>130</v>
       </c>
       <c r="F36" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -43274,7 +43478,7 @@
         <v>131</v>
       </c>
       <c r="F37" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -43294,7 +43498,7 @@
         <v>132</v>
       </c>
       <c r="F38" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -43314,7 +43518,7 @@
         <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -43334,7 +43538,7 @@
         <v>133</v>
       </c>
       <c r="F40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -43354,7 +43558,7 @@
         <v>150</v>
       </c>
       <c r="F41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -43374,7 +43578,7 @@
         <v>140</v>
       </c>
       <c r="F42" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -43394,7 +43598,7 @@
         <v>113</v>
       </c>
       <c r="F43" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -43414,7 +43618,7 @@
         <v>134</v>
       </c>
       <c r="F44" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -43434,7 +43638,189 @@
         <v>115</v>
       </c>
       <c r="F45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B1" s="115" t="s">
         <v>195</v>
+      </c>
+      <c r="C1" s="115" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="115">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="115">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="115">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="115">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="115">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="115">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="115">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="115">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="115">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="115">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="115">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="115">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="115">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="115">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -45680,8 +46066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AS40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -45733,12 +46119,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="84" customFormat="1" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="132"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="135"/>
     </row>
     <row r="2" spans="1:39" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="95" t="s">
@@ -46102,10 +46488,10 @@
       <c r="H5" s="82"/>
     </row>
     <row r="6" spans="1:39" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="136" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="124"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="84"/>
     </row>
     <row r="7" spans="1:39" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -46172,12 +46558,12 @@
     </row>
     <row r="14" spans="1:39" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="15" spans="1:39" s="101" customFormat="1" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A15" s="130" t="s">
+      <c r="A15" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="132"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="135"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A16" s="103" t="s">
@@ -46520,11 +46906,11 @@
     </row>
     <row r="19" spans="1:45" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="20" spans="1:45" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A20" s="133" t="str">
+      <c r="A20" s="136" t="str">
         <f>A6</f>
         <v>Metrics</v>
       </c>
-      <c r="B20" s="124"/>
+      <c r="B20" s="127"/>
     </row>
     <row r="21" spans="1:45" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="91" t="str">
@@ -46574,12 +46960,12 @@
     </row>
     <row r="26" spans="1:45" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="27" spans="1:45" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A27" s="130" t="s">
+      <c r="A27" s="133" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
-      <c r="D27" s="132"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="135"/>
     </row>
     <row r="28" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="90" t="str">
@@ -46999,11 +47385,11 @@
       <c r="A31" s="86"/>
     </row>
     <row r="32" spans="1:45" ht="21.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A32" s="134" t="str">
+      <c r="A32" s="137" t="str">
         <f>A20</f>
         <v>Metrics</v>
       </c>
-      <c r="B32" s="124"/>
+      <c r="B32" s="127"/>
     </row>
     <row r="33" spans="1:2" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="93" t="str">

</xml_diff>